<commit_message>
making a big changes to this branch
</commit_message>
<xml_diff>
--- a/dummy.xlsx
+++ b/dummy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\crud-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78930EC7-0F16-41AC-908C-D64760D5933D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77606D53-F605-4322-8ED9-C83737985C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2760" yWindow="3348" windowWidth="17280" windowHeight="8880" xr2:uid="{3ABC5DD1-D8CA-4439-9657-A721D95F93CF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="5">
   <si>
     <t>TI-2B</t>
   </si>
@@ -402,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{983AE3DD-B07A-4F37-BE94-424E64D48C07}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -758,6 +758,354 @@
         <v>3</v>
       </c>
     </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>2020</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="I13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>2020</v>
+      </c>
+      <c r="H14">
+        <v>4</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>2020</v>
+      </c>
+      <c r="H15">
+        <v>4</v>
+      </c>
+      <c r="I15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>2020</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>2020</v>
+      </c>
+      <c r="H17">
+        <v>4</v>
+      </c>
+      <c r="I17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>2020</v>
+      </c>
+      <c r="H18">
+        <v>4</v>
+      </c>
+      <c r="I18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>2020</v>
+      </c>
+      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="I19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>2020</v>
+      </c>
+      <c r="H20">
+        <v>4</v>
+      </c>
+      <c r="I20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>2020</v>
+      </c>
+      <c r="H21">
+        <v>4</v>
+      </c>
+      <c r="I21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>2020</v>
+      </c>
+      <c r="H22">
+        <v>4</v>
+      </c>
+      <c r="I22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>2020</v>
+      </c>
+      <c r="H23">
+        <v>4</v>
+      </c>
+      <c r="I23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>2020</v>
+      </c>
+      <c r="H24">
+        <v>4</v>
+      </c>
+      <c r="I24">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>